<commit_message>
Relative path for file
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="570" windowWidth="14055" windowHeight="6090" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14340" windowHeight="2985" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Saturday" sheetId="1" r:id="rId1"/>
@@ -16,11 +16,12 @@
     <sheet name="Friday" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:J8"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="60">
   <si>
     <t>Longest Option</t>
   </si>
@@ -167,17 +168,60 @@
     <t>hello world</t>
   </si>
   <si>
-    <t>xshell download for windows 10</t>
-  </si>
-  <si>
-    <t>xshell</t>
+    <t>cricket live score today</t>
+  </si>
+  <si>
+    <t>money heist season 6 release date</t>
+  </si>
+  <si>
+    <t>money</t>
+  </si>
+  <si>
+    <t>inter milan vs atletico madrid</t>
+  </si>
+  <si>
+    <t>inter miami vs</t>
+  </si>
+  <si>
+    <t>goods meaning in bengali
+পণ্য (Bangla)</t>
+  </si>
+  <si>
+    <t>goods</t>
+  </si>
+  <si>
+    <t>dhaka education board
+Board of Intermediate and Secondary Education, Dhaka · 5 Joynag Rd, Dhaka</t>
+  </si>
+  <si>
+    <t>sunday suspense sherlock holmes</t>
+  </si>
+  <si>
+    <t>sunday</t>
+  </si>
+  <si>
+    <t>baby pic</t>
+  </si>
+  <si>
+    <t>cricket icc
+International Cricket Council — Cricket administrative body</t>
+  </si>
+  <si>
+    <t>money heist berlin series</t>
+  </si>
+  <si>
+    <t>International Cricket Council
+Cricket administrative body</t>
+  </si>
+  <si>
+    <t>Looking
+American comedy-drama series</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -562,7 +606,7 @@
   </sheetPr>
   <dimension ref="B2:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -581,6 +625,12 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
@@ -589,6 +639,12 @@
       <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
@@ -597,6 +653,12 @@
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -605,6 +667,12 @@
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
@@ -613,6 +681,12 @@
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
@@ -621,6 +695,12 @@
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
@@ -629,6 +709,12 @@
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
@@ -637,6 +723,12 @@
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="D10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
@@ -644,6 +736,12 @@
       </c>
       <c r="C11" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
@@ -666,7 +764,7 @@
   </sheetPr>
   <dimension ref="B2:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -770,7 +868,7 @@
   </sheetPr>
   <dimension ref="B2:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -876,7 +974,7 @@
   </sheetPr>
   <dimension ref="B2:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -895,10 +993,10 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -909,10 +1007,10 @@
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>30</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -923,10 +1021,10 @@
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>32</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -937,10 +1035,10 @@
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>34</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E6" t="s">
         <v>35</v>
       </c>
     </row>
@@ -951,10 +1049,10 @@
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>36</v>
       </c>
-      <c r="E7" t="s" s="0">
+      <c r="E7" t="s">
         <v>37</v>
       </c>
     </row>
@@ -965,10 +1063,10 @@
       <c r="C8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>38</v>
       </c>
-      <c r="E8" t="s" s="0">
+      <c r="E8" t="s">
         <v>25</v>
       </c>
     </row>
@@ -979,10 +1077,10 @@
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="D9" t="s">
         <v>39</v>
       </c>
-      <c r="E9" t="s" s="0">
+      <c r="E9" t="s">
         <v>40</v>
       </c>
     </row>
@@ -993,10 +1091,10 @@
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" t="s" s="0">
+      <c r="D10" t="s">
         <v>41</v>
       </c>
-      <c r="E10" t="s" s="0">
+      <c r="E10" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1007,10 +1105,10 @@
       <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>43</v>
       </c>
-      <c r="E11" t="s" s="0">
+      <c r="E11" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1034,7 +1132,7 @@
   </sheetPr>
   <dimension ref="B2:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1053,6 +1151,12 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
@@ -1061,6 +1165,12 @@
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
@@ -1069,6 +1179,12 @@
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -1077,6 +1193,12 @@
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
@@ -1085,6 +1207,12 @@
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
@@ -1093,6 +1221,12 @@
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
@@ -1101,6 +1235,12 @@
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
@@ -1109,6 +1249,12 @@
       <c r="C10" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
@@ -1116,6 +1262,12 @@
       </c>
       <c r="C11" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
@@ -1142,10 +1294,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" customWidth="true" width="10.140625"/>
-    <col min="4" max="4" customWidth="true" width="8.140625"/>
-    <col min="5" max="5" customWidth="true" width="8.28515625"/>
-    <col min="6" max="6" customWidth="true" width="5.0"/>
+    <col min="2" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" customWidth="1"/>
+    <col min="6" max="6" width="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>